<commit_message>
Add Jupyter Notebook for Aggregation and Grouping Analysis
- Created a new Jupyter Notebook (07_Aggregration & Grouping.ipynb) to demonstrate various aggregation and grouping techniques using pandas.
- Included data creation, groupby operations, and aggregation functions such as mean, max, min, and count.
- Added a new column for team averages and filtered teams based on salary criteria.

Also, added a temporary Excel file for data storage.
</commit_message>
<xml_diff>
--- a/anaconda_projects/db/data.xlsx
+++ b/anaconda_projects/db/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suman Pradhan\OneDrive\Desktop\Data Science\PANDAS\anaconda_projects\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8306B1D6-8875-4EE2-B0B0-0E4ED5B757F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF0C16-7377-4E14-B5A6-4A17B2331839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11592" yWindow="1044" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="3024" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Actor</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Biopic</t>
+  </si>
+  <si>
+    <t>IMDB</t>
   </si>
 </sst>
 </file>
@@ -423,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +450,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -464,8 +470,11 @@
       <c r="E2">
         <v>1050</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -481,8 +490,11 @@
       <c r="E3">
         <v>565</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -498,8 +510,11 @@
       <c r="E4">
         <v>2024</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -515,8 +530,11 @@
       <c r="E5">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -532,8 +550,11 @@
       <c r="E6">
         <v>475</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -549,8 +570,11 @@
       <c r="E7">
         <v>431</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -566,8 +590,11 @@
       <c r="E8">
         <v>318</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -582,6 +609,9 @@
       </c>
       <c r="E9">
         <v>525</v>
+      </c>
+      <c r="F9">
+        <v>6.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>